<commit_message>
Modules are developed and tested for orbital element conversions, through Canvas
</commit_message>
<xml_diff>
--- a/Laboratory/Ideas.xlsx
+++ b/Laboratory/Ideas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3189723E-399A-4C95-85A7-B3E1E4CE1440}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C006ADD-7D1A-40CE-AE9D-65D80B8178C8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>MGOD course</t>
   </si>
@@ -165,10 +165,17 @@
     <t>Status in  MoMPy</t>
   </si>
   <si>
-    <t>WIP</t>
-  </si>
-  <si>
     <t>Page 22 of LN</t>
+  </si>
+  <si>
+    <t>Version details</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>1. Basics-I.py (Base and original assignment)
+2. Basics-I_ver1.py (Next version, functions introduced)</t>
   </si>
 </sst>
 </file>
@@ -293,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -323,6 +330,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -617,9 +630,10 @@
     <col min="4" max="4" width="23.7265625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="16.453125" customWidth="1"/>
+    <col min="7" max="7" width="50.08984375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -629,7 +643,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -648,8 +662,11 @@
       <c r="F2" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -660,8 +677,9 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
@@ -672,16 +690,19 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -690,8 +711,9 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
       <c r="B6" s="1" t="s">
         <v>10</v>
@@ -702,8 +724,9 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -716,8 +739,9 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="10"/>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -730,8 +754,9 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
         <v>18</v>
@@ -744,8 +769,9 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="10"/>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -760,8 +786,9 @@
       <c r="F10" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
       <c r="B11" s="1" t="s">
         <v>23</v>
@@ -772,8 +799,9 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="10"/>
       <c r="B12" s="1" t="s">
         <v>24</v>
@@ -784,8 +812,9 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="10"/>
       <c r="B13" s="1" t="s">
         <v>26</v>
@@ -796,8 +825,9 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="10"/>
       <c r="B14" s="1" t="s">
         <v>28</v>
@@ -808,8 +838,9 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="10"/>
       <c r="B15" s="1" t="s">
         <v>30</v>
@@ -820,8 +851,9 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="10"/>
       <c r="B16" s="1" t="s">
         <v>32</v>
@@ -834,8 +866,9 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="10"/>
       <c r="B17" s="1" t="s">
         <v>34</v>
@@ -846,8 +879,9 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="10"/>
       <c r="B18" s="1" t="s">
         <v>36</v>
@@ -858,8 +892,9 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="10"/>
       <c r="B19" s="4" t="s">
         <v>38</v>
@@ -870,8 +905,9 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="10"/>
       <c r="B20" s="4" t="s">
         <v>40</v>
@@ -882,8 +918,9 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
       <c r="B21" s="4" t="s">
         <v>42</v>
@@ -894,6 +931,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
+      <c r="G21" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
After ideas sheet updated, pygmo installed.
</commit_message>
<xml_diff>
--- a/Laboratory/Ideas.xlsx
+++ b/Laboratory/Ideas.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECD456D-3CC9-478B-907B-247FC0200FBD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084866D6-B39F-471B-A393-EAA9646C9BFA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TU Delft courses" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Other" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>MGOD course</t>
   </si>
@@ -175,7 +175,32 @@
   </si>
   <si>
     <t>1. Basics-I.py (Base and original assignment)
-2. Basics-I_ver1.py (Next version, functions introduced)</t>
+2. Basics-I_ver1.py (Next version, functions introduced)
+3. Modules created and added to BasicAstrodynamics.py and tested through Canvas.py</t>
+  </si>
+  <si>
+    <t>Sr.No</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Installation of spiceypy</t>
+  </si>
+  <si>
+    <t>Installation of pygmo</t>
+  </si>
+  <si>
+    <t>Tested through Pygmo_test.py</t>
+  </si>
+  <si>
+    <t>Tested through Canvas.py</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -300,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -310,6 +335,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -331,11 +362,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -620,7 +657,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -630,18 +667,18 @@
     <col min="4" max="4" width="23.7265625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="16.453125" customWidth="1"/>
-    <col min="7" max="7" width="50.08984375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="50.08984375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -662,7 +699,7 @@
       <c r="F2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="6" t="s">
         <v>48</v>
       </c>
     </row>
@@ -679,14 +716,14 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:7" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -703,18 +740,18 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="7"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -727,7 +764,7 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="10"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
@@ -742,7 +779,7 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="10"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
@@ -757,7 +794,7 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
@@ -772,7 +809,7 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
@@ -789,7 +826,7 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
@@ -802,7 +839,7 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="10"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
@@ -815,7 +852,7 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
@@ -828,7 +865,7 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
@@ -841,7 +878,7 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
@@ -854,7 +891,7 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
@@ -869,7 +906,7 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
@@ -882,7 +919,7 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="10"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -895,7 +932,7 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="10"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="4" t="s">
         <v>38</v>
       </c>
@@ -908,7 +945,7 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="10"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="4" t="s">
         <v>40</v>
       </c>
@@ -921,7 +958,7 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="4" t="s">
         <v>42</v>
       </c>
@@ -945,12 +982,102 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD8FA87-E19D-4B8B-8DE8-AF98BD485E94}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="36.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14">
+        <v>43781</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="13"/>
+      <c r="B4" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5" s="15">
+        <v>43787</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="13"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A3:A4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
After base version for assignment basics07 is complete
</commit_message>
<xml_diff>
--- a/Laboratory/Ideas.xlsx
+++ b/Laboratory/Ideas.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084866D6-B39F-471B-A393-EAA9646C9BFA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0BEB22-8C18-4DAD-9D73-DABCCAC39EC8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>MGOD course</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>Status in  MoMPy</t>
@@ -201,6 +198,12 @@
   </si>
   <si>
     <t>??</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>1. Basics-VII.py (Base and original assignment)</t>
   </si>
 </sst>
 </file>
@@ -341,6 +344,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -362,16 +371,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -656,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -671,14 +674,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -697,10 +700,10 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -717,41 +720,41 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="12"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -764,7 +767,7 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
@@ -779,7 +782,7 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
@@ -794,7 +797,7 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="12"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
@@ -809,7 +812,7 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="12"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
@@ -821,12 +824,14 @@
         <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="12"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
@@ -839,7 +844,7 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="12"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
@@ -852,7 +857,7 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="12"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
@@ -865,7 +870,7 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
@@ -878,7 +883,7 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
@@ -891,7 +896,7 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
@@ -906,7 +911,7 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
@@ -919,7 +924,7 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -932,7 +937,7 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="12"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="4" t="s">
         <v>38</v>
       </c>
@@ -945,7 +950,7 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="12"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="4" t="s">
         <v>40</v>
       </c>
@@ -958,7 +963,7 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="13"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="4" t="s">
         <v>42</v>
       </c>
@@ -995,51 +1000,51 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>43781</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="11">
-        <v>1</v>
-      </c>
-      <c r="B3" s="14">
-        <v>43781</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="15"/>
+      <c r="B4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="13">
+        <v>2</v>
+      </c>
+      <c r="B5" s="16">
+        <v>43787</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="13"/>
-      <c r="B4" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="11">
-        <v>2</v>
-      </c>
-      <c r="B5" s="15">
-        <v>43787</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="15"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
After testing modules for ER orbits at all three runs, no results are plotted
</commit_message>
<xml_diff>
--- a/Laboratory/Ideas.xlsx
+++ b/Laboratory/Ideas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0BEB22-8C18-4DAD-9D73-DABCCAC39EC8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8015F06F-6B7C-4413-8823-287F85702932}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t>MGOD course</t>
   </si>
@@ -200,18 +200,171 @@
     <t>??</t>
   </si>
   <si>
-    <t>WIP</t>
-  </si>
-  <si>
-    <t>1. Basics-VII.py (Base and original assignment)</t>
+    <t>Future scope</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>After Basics-I_ver1.py:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Define the import of required modules within function</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1. After Basics-VII_ver1.py :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+i. Extract </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>all</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> useful parameters from SPICE
+ii. Remove extra steps in low fidelity + unknown inclination case, to find cosine inverse. Two </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> conditions should do.
+iii. Add steps for low fidelity + unknown altitude case
+iv. Return an extra variable as a map of rows where the solutions are stored</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. Basics-VII.py (Base and original assignment)
+2. Basics-VII_ver1.py (Next version, functions introduced)
+3. Modules created and added to OrbitDesign.py and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">tested through Canvas.py </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Test by plotting is left)</t>
+    </r>
+  </si>
+  <si>
+    <t>Zero eccentricity ER orbits solutions to be found</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -328,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -341,9 +494,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -376,6 +526,12 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,33 +813,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11.36328125" customWidth="1"/>
-    <col min="3" max="3" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="32.08984375" customWidth="1"/>
     <col min="4" max="4" width="23.7265625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="16.453125" customWidth="1"/>
     <col min="7" max="7" width="50.08984375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="44.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+      <c r="H1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -702,11 +862,12 @@
       <c r="F2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="17" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -717,16 +878,17 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="G3" s="18"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -738,23 +900,27 @@
       <c r="F4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
+      <c r="H4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="13"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="14"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="13"/>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -764,10 +930,11 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="14"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="13"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
@@ -779,10 +946,11 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="14"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="13"/>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
@@ -794,10 +962,11 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="13"/>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
@@ -809,29 +978,35 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="14"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="13"/>
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="14"/>
+        <v>48</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="13"/>
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
@@ -843,8 +1018,8 @@
       <c r="F11" s="1"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="14"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="13"/>
       <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
@@ -856,8 +1031,8 @@
       <c r="F12" s="1"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="14"/>
+    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="13"/>
       <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
@@ -869,8 +1044,8 @@
       <c r="F13" s="1"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="13"/>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
@@ -882,8 +1057,8 @@
       <c r="F14" s="1"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="13"/>
       <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
@@ -895,8 +1070,8 @@
       <c r="F15" s="1"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
+    <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="13"/>
       <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
@@ -911,7 +1086,7 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
@@ -924,7 +1099,7 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="14"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -937,7 +1112,7 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="4" t="s">
         <v>38</v>
       </c>
@@ -950,7 +1125,7 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="4" t="s">
         <v>40</v>
       </c>
@@ -963,7 +1138,7 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="15"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="4" t="s">
         <v>42</v>
       </c>
@@ -982,6 +1157,7 @@
     <mergeCell ref="A4:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1010,10 +1186,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>43781</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1021,8 +1197,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="15"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1030,10 +1206,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>2</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="15">
         <v>43787</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1041,8 +1217,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
-      <c r="B6" s="17"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="1" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Added future scopes for the scripts developed so far
</commit_message>
<xml_diff>
--- a/Laboratory/Ideas.xlsx
+++ b/Laboratory/Ideas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8015F06F-6B7C-4413-8823-287F85702932}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434A0C44-FAB8-41A5-A803-21854737AEF2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>